<commit_message>
Refactored scripts for sales contract
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager_Sale_Contract.xlsx
+++ b/src/test/resources/Run_Manager_Sale_Contract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\New_Sakani_TST_Git\Sakani_TST_New\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F43A6C1-3EBC-4D93-8454-3FA368A1CC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88C6665-63AF-4645-86E9-98761F8F82C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -653,9 +653,6 @@
     <t>Complete unit booking and pay the booking fee</t>
   </si>
   <si>
-    <t>Get the unit code of booked unit</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify Booking fee status is paid </t>
   </si>
   <si>
@@ -1883,6 +1880,9 @@
       </rPr>
       <t xml:space="preserve"> and save the project</t>
     </r>
+  </si>
+  <si>
+    <t>Approve the sign contract</t>
   </si>
 </sst>
 </file>
@@ -2701,8 +2701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="C16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65:J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2808,13 +2808,13 @@
         <v>27</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>50</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>15</v>
@@ -2823,7 +2823,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K3" s="13">
         <v>1</v>
@@ -2847,13 +2847,13 @@
         <v>28</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>15</v>
@@ -2862,7 +2862,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K4" s="13">
         <v>1</v>
@@ -2886,13 +2886,13 @@
         <v>29</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>15</v>
@@ -2901,7 +2901,7 @@
         <v>16</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K5" s="13">
         <v>1</v>
@@ -2925,13 +2925,13 @@
         <v>30</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>15</v>
@@ -2940,7 +2940,7 @@
         <v>16</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K6" s="13">
         <v>1</v>
@@ -2964,13 +2964,13 @@
         <v>31</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>15</v>
@@ -2979,7 +2979,7 @@
         <v>16</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K7" s="13">
         <v>1</v>
@@ -3003,13 +3003,13 @@
         <v>32</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>15</v>
@@ -3018,7 +3018,7 @@
         <v>16</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K8" s="13">
         <v>1</v>
@@ -3042,13 +3042,13 @@
         <v>33</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>15</v>
@@ -3057,7 +3057,7 @@
         <v>16</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K9" s="13">
         <v>1</v>
@@ -3081,13 +3081,13 @@
         <v>34</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>15</v>
@@ -3096,7 +3096,7 @@
         <v>16</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K10" s="13">
         <v>1</v>
@@ -3120,13 +3120,13 @@
         <v>35</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>15</v>
@@ -3135,7 +3135,7 @@
         <v>16</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K11" s="13">
         <v>1</v>
@@ -3159,13 +3159,13 @@
         <v>36</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>15</v>
@@ -3174,7 +3174,7 @@
         <v>16</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K12" s="13">
         <v>1</v>
@@ -3198,13 +3198,13 @@
         <v>37</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>15</v>
@@ -3213,7 +3213,7 @@
         <v>16</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K13" s="13">
         <v>1</v>
@@ -3237,13 +3237,13 @@
         <v>38</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H14" s="13" t="s">
         <v>15</v>
@@ -3252,7 +3252,7 @@
         <v>16</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K14" s="13">
         <v>1</v>
@@ -3276,13 +3276,13 @@
         <v>39</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>15</v>
@@ -3291,7 +3291,7 @@
         <v>16</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K15" s="13">
         <v>1</v>
@@ -3315,13 +3315,13 @@
         <v>40</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H16" s="13" t="s">
         <v>15</v>
@@ -3330,7 +3330,7 @@
         <v>16</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K16" s="13">
         <v>1</v>
@@ -3385,13 +3385,13 @@
         <v>46</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H18" s="13" t="s">
         <v>15</v>
@@ -3400,7 +3400,7 @@
         <v>16</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K18" s="13">
         <v>1</v>
@@ -3424,13 +3424,13 @@
         <v>47</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>50</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>15</v>
@@ -3439,7 +3439,7 @@
         <v>16</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K19" s="13">
         <v>1</v>
@@ -3457,19 +3457,19 @@
         <v>45</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H20" s="13" t="s">
         <v>15</v>
@@ -3478,7 +3478,7 @@
         <v>16</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K20" s="13">
         <v>1</v>
@@ -3496,19 +3496,19 @@
         <v>45</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>50</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H21" s="13" t="s">
         <v>15</v>
@@ -3517,7 +3517,7 @@
         <v>16</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K21" s="13">
         <v>1</v>
@@ -3541,13 +3541,13 @@
         <v>48</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>50</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H22" s="13" t="s">
         <v>15</v>
@@ -3556,7 +3556,7 @@
         <v>16</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K22" s="13">
         <v>1</v>
@@ -3580,13 +3580,13 @@
         <v>49</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>50</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>15</v>
@@ -3595,7 +3595,7 @@
         <v>16</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K23" s="13">
         <v>1</v>
@@ -3613,7 +3613,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="22" t="s">
@@ -3641,22 +3641,22 @@
         <v>21</v>
       </c>
       <c r="B25" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="C25" s="23" t="s">
         <v>342</v>
       </c>
-      <c r="C25" s="23" t="s">
-        <v>343</v>
-      </c>
       <c r="D25" s="23" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H25" s="13" t="s">
         <v>15</v>
@@ -3665,7 +3665,7 @@
         <v>16</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K25" s="13">
         <v>1</v>
@@ -3680,22 +3680,22 @@
         <v>22</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>15</v>
@@ -3704,7 +3704,7 @@
         <v>16</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K26" s="13">
         <v>1</v>
@@ -3719,22 +3719,22 @@
         <v>23</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H27" s="13" t="s">
         <v>15</v>
@@ -3743,7 +3743,7 @@
         <v>16</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K27" s="13">
         <v>1</v>
@@ -3798,13 +3798,13 @@
         <v>54</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H29" s="13" t="s">
         <v>15</v>
@@ -3813,7 +3813,7 @@
         <v>16</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="K29" s="13">
         <v>1</v>
@@ -3831,19 +3831,19 @@
         <v>53</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H30" s="13" t="s">
         <v>15</v>
@@ -3852,7 +3852,7 @@
         <v>16</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="K30" s="13">
         <v>1</v>
@@ -3870,19 +3870,19 @@
         <v>53</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>55</v>
+        <v>370</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>55</v>
+        <v>370</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>15</v>
@@ -3891,7 +3891,7 @@
         <v>16</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="K31" s="13">
         <v>1</v>
@@ -3903,13 +3903,13 @@
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="22" t="s">
@@ -3937,22 +3937,22 @@
         <v>27</v>
       </c>
       <c r="B33" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="19" t="s">
-        <v>59</v>
-      </c>
       <c r="D33" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>15</v>
@@ -3961,7 +3961,7 @@
         <v>16</v>
       </c>
       <c r="J33" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K33" s="13">
         <v>1</v>
@@ -3976,22 +3976,22 @@
         <v>28</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>15</v>
@@ -4000,7 +4000,7 @@
         <v>16</v>
       </c>
       <c r="J34" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K34" s="13">
         <v>1</v>
@@ -4015,22 +4015,22 @@
         <v>29</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H35" s="13" t="s">
         <v>15</v>
@@ -4039,7 +4039,7 @@
         <v>16</v>
       </c>
       <c r="J35" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K35" s="13">
         <v>1</v>
@@ -4054,22 +4054,22 @@
         <v>30</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>15</v>
@@ -4078,7 +4078,7 @@
         <v>16</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K36" s="13">
         <v>1</v>
@@ -4093,22 +4093,22 @@
         <v>31</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H37" s="13" t="s">
         <v>15</v>
@@ -4117,7 +4117,7 @@
         <v>16</v>
       </c>
       <c r="J37" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K37" s="13">
         <v>1</v>
@@ -4132,22 +4132,22 @@
         <v>32</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H38" s="13" t="s">
         <v>15</v>
@@ -4156,7 +4156,7 @@
         <v>16</v>
       </c>
       <c r="J38" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K38" s="13">
         <v>1</v>
@@ -4168,13 +4168,13 @@
     </row>
     <row r="39" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="22" t="s">
@@ -4202,22 +4202,22 @@
         <v>33</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H40" s="13" t="s">
         <v>15</v>
@@ -4226,7 +4226,7 @@
         <v>16</v>
       </c>
       <c r="J40" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K40" s="13">
         <v>1</v>
@@ -4241,22 +4241,22 @@
         <v>34</v>
       </c>
       <c r="B41" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="D41" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H41" s="13" t="s">
         <v>15</v>
@@ -4265,7 +4265,7 @@
         <v>16</v>
       </c>
       <c r="J41" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K41" s="13">
         <v>1</v>
@@ -4280,22 +4280,22 @@
         <v>35</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F42" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H42" s="13" t="s">
         <v>15</v>
@@ -4304,7 +4304,7 @@
         <v>16</v>
       </c>
       <c r="J42" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K42" s="13">
         <v>1</v>
@@ -4319,22 +4319,22 @@
         <v>36</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F43" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H43" s="13" t="s">
         <v>15</v>
@@ -4343,7 +4343,7 @@
         <v>16</v>
       </c>
       <c r="J43" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K43" s="13">
         <v>1</v>
@@ -4358,22 +4358,22 @@
         <v>37</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F44" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H44" s="13" t="s">
         <v>15</v>
@@ -4382,7 +4382,7 @@
         <v>16</v>
       </c>
       <c r="J44" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K44" s="13">
         <v>1</v>
@@ -4397,22 +4397,22 @@
         <v>38</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>15</v>
@@ -4421,7 +4421,7 @@
         <v>16</v>
       </c>
       <c r="J45" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K45" s="13">
         <v>1</v>
@@ -4436,22 +4436,22 @@
         <v>39</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H46" s="13" t="s">
         <v>15</v>
@@ -4460,7 +4460,7 @@
         <v>16</v>
       </c>
       <c r="J46" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K46" s="13">
         <v>1</v>
@@ -4475,22 +4475,22 @@
         <v>40</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F47" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H47" s="13" t="s">
         <v>15</v>
@@ -4499,7 +4499,7 @@
         <v>16</v>
       </c>
       <c r="J47" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K47" s="13">
         <v>1</v>
@@ -4514,22 +4514,22 @@
         <v>41</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F48" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H48" s="13" t="s">
         <v>15</v>
@@ -4538,7 +4538,7 @@
         <v>16</v>
       </c>
       <c r="J48" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K48" s="13">
         <v>1</v>
@@ -4553,22 +4553,22 @@
         <v>42</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F49" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H49" s="13" t="s">
         <v>15</v>
@@ -4577,7 +4577,7 @@
         <v>16</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K49" s="13">
         <v>1</v>
@@ -4592,22 +4592,22 @@
         <v>43</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F50" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H50" s="13" t="s">
         <v>15</v>
@@ -4616,7 +4616,7 @@
         <v>16</v>
       </c>
       <c r="J50" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K50" s="13">
         <v>1</v>
@@ -4631,22 +4631,22 @@
         <v>44</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F51" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H51" s="13" t="s">
         <v>15</v>
@@ -4655,7 +4655,7 @@
         <v>16</v>
       </c>
       <c r="J51" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K51" s="13">
         <v>1</v>
@@ -4670,22 +4670,22 @@
         <v>45</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F52" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H52" s="13" t="s">
         <v>15</v>
@@ -4694,7 +4694,7 @@
         <v>16</v>
       </c>
       <c r="J52" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K52" s="13">
         <v>1</v>
@@ -4709,22 +4709,22 @@
         <v>46</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F53" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H53" s="13" t="s">
         <v>15</v>
@@ -4733,7 +4733,7 @@
         <v>16</v>
       </c>
       <c r="J53" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K53" s="13">
         <v>1</v>
@@ -4748,22 +4748,22 @@
         <v>47</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F54" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H54" s="13" t="s">
         <v>15</v>
@@ -4772,7 +4772,7 @@
         <v>16</v>
       </c>
       <c r="J54" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K54" s="13">
         <v>1</v>
@@ -4787,22 +4787,22 @@
         <v>48</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F55" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G55" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H55" s="13" t="s">
         <v>15</v>
@@ -4811,7 +4811,7 @@
         <v>16</v>
       </c>
       <c r="J55" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K55" s="13">
         <v>1</v>
@@ -4826,22 +4826,22 @@
         <v>49</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H56" s="13" t="s">
         <v>15</v>
@@ -4850,7 +4850,7 @@
         <v>16</v>
       </c>
       <c r="J56" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K56" s="13">
         <v>1</v>
@@ -4865,22 +4865,22 @@
         <v>50</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F57" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H57" s="13" t="s">
         <v>15</v>
@@ -4889,7 +4889,7 @@
         <v>16</v>
       </c>
       <c r="J57" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K57" s="13">
         <v>1</v>
@@ -4904,22 +4904,22 @@
         <v>51</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F58" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H58" s="13" t="s">
         <v>15</v>
@@ -4928,7 +4928,7 @@
         <v>16</v>
       </c>
       <c r="J58" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K58" s="13">
         <v>1</v>
@@ -4937,7 +4937,7 @@
         <v>51</v>
       </c>
       <c r="M58" s="32" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -4945,22 +4945,22 @@
         <v>52</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F59" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H59" s="13" t="s">
         <v>15</v>
@@ -4969,7 +4969,7 @@
         <v>16</v>
       </c>
       <c r="J59" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K59" s="13">
         <v>1</v>
@@ -4981,13 +4981,13 @@
     </row>
     <row r="60" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="22" t="s">
@@ -5015,22 +5015,22 @@
         <v>53</v>
       </c>
       <c r="B61" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="D61" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F61" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H61" s="13" t="s">
         <v>15</v>
@@ -5039,7 +5039,7 @@
         <v>16</v>
       </c>
       <c r="J61" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K61" s="13">
         <v>1</v>
@@ -5054,22 +5054,22 @@
         <v>54</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F62" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H62" s="13" t="s">
         <v>15</v>
@@ -5078,7 +5078,7 @@
         <v>16</v>
       </c>
       <c r="J62" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K62" s="13">
         <v>1</v>
@@ -5093,22 +5093,22 @@
         <v>55</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F63" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H63" s="13" t="s">
         <v>15</v>
@@ -5117,7 +5117,7 @@
         <v>16</v>
       </c>
       <c r="J63" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K63" s="13">
         <v>1</v>
@@ -5129,13 +5129,13 @@
     </row>
     <row r="64" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="22" t="s">
@@ -5163,22 +5163,22 @@
         <v>56</v>
       </c>
       <c r="B65" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C65" s="12" t="s">
-        <v>93</v>
-      </c>
       <c r="D65" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H65" s="13" t="s">
         <v>15</v>
@@ -5187,7 +5187,7 @@
         <v>16</v>
       </c>
       <c r="J65" s="14" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="K65" s="13">
         <v>1</v>
@@ -5202,22 +5202,22 @@
         <v>57</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H66" s="13" t="s">
         <v>15</v>
@@ -5226,7 +5226,7 @@
         <v>16</v>
       </c>
       <c r="J66" s="14" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="K66" s="13">
         <v>1</v>
@@ -5241,22 +5241,22 @@
         <v>58</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H67" s="13" t="s">
         <v>15</v>
@@ -5265,7 +5265,7 @@
         <v>16</v>
       </c>
       <c r="J67" s="14" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="K67" s="13">
         <v>1</v>
@@ -5280,22 +5280,22 @@
         <v>59</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G68" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H68" s="13" t="s">
         <v>15</v>
@@ -5304,7 +5304,7 @@
         <v>16</v>
       </c>
       <c r="J68" s="14" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="K68" s="13">
         <v>1</v>
@@ -5319,22 +5319,22 @@
         <v>60</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G69" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H69" s="13" t="s">
         <v>15</v>
@@ -5343,7 +5343,7 @@
         <v>16</v>
       </c>
       <c r="J69" s="14" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="K69" s="13">
         <v>1</v>
@@ -5358,22 +5358,22 @@
         <v>61</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H70" s="13" t="s">
         <v>15</v>
@@ -5382,7 +5382,7 @@
         <v>16</v>
       </c>
       <c r="J70" s="14" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="K70" s="13">
         <v>1</v>
@@ -5397,22 +5397,22 @@
         <v>62</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F71" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H71" s="13" t="s">
         <v>15</v>
@@ -5421,7 +5421,7 @@
         <v>16</v>
       </c>
       <c r="J71" s="14" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="K71" s="13">
         <v>1</v>
@@ -5436,22 +5436,22 @@
         <v>63</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F72" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G72" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H72" s="13" t="s">
         <v>15</v>
@@ -5460,7 +5460,7 @@
         <v>16</v>
       </c>
       <c r="J72" s="14" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="K72" s="13">
         <v>1</v>
@@ -5475,22 +5475,22 @@
         <v>64</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C73" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="D73" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="D73" s="12" t="s">
-        <v>337</v>
-      </c>
       <c r="E73" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F73" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G73" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H73" s="13" t="s">
         <v>15</v>
@@ -5499,7 +5499,7 @@
         <v>16</v>
       </c>
       <c r="J73" s="14" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="K73" s="13">
         <v>1</v>
@@ -5511,13 +5511,13 @@
     </row>
     <row r="74" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D74" s="8"/>
       <c r="E74" s="22" t="s">
@@ -5545,22 +5545,22 @@
         <v>65</v>
       </c>
       <c r="B75" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C75" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C75" s="23" t="s">
-        <v>102</v>
-      </c>
       <c r="D75" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F75" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G75" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H75" s="13" t="s">
         <v>15</v>
@@ -5569,7 +5569,7 @@
         <v>16</v>
       </c>
       <c r="J75" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K75" s="13">
         <v>1</v>
@@ -5584,22 +5584,22 @@
         <v>66</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D76" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F76" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G76" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H76" s="13" t="s">
         <v>15</v>
@@ -5608,7 +5608,7 @@
         <v>16</v>
       </c>
       <c r="J76" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K76" s="13">
         <v>1</v>
@@ -5623,22 +5623,22 @@
         <v>67</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D77" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G77" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H77" s="13" t="s">
         <v>15</v>
@@ -5647,7 +5647,7 @@
         <v>16</v>
       </c>
       <c r="J77" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K77" s="13">
         <v>1</v>
@@ -5662,22 +5662,22 @@
         <v>68</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C78" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D78" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F78" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G78" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H78" s="13" t="s">
         <v>15</v>
@@ -5686,7 +5686,7 @@
         <v>16</v>
       </c>
       <c r="J78" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K78" s="13">
         <v>1</v>
@@ -5701,22 +5701,22 @@
         <v>69</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C79" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D79" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G79" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H79" s="13" t="s">
         <v>15</v>
@@ -5725,7 +5725,7 @@
         <v>16</v>
       </c>
       <c r="J79" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K79" s="13">
         <v>1</v>
@@ -5740,22 +5740,22 @@
         <v>70</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D80" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F80" s="12" t="s">
         <v>42</v>
       </c>
       <c r="G80" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H80" s="13" t="s">
         <v>15</v>
@@ -5764,7 +5764,7 @@
         <v>16</v>
       </c>
       <c r="J80" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K80" s="13">
         <v>1</v>
@@ -5879,7 +5879,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J25:J27 J18:J23 J40:J59 J65:J73 J3:J16 J75:J80 J33:J38 J61:J63 J29:J31" xr:uid="{94536AF8-B0B3-4690-A59B-64F66E932AAC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J25:J27 J18:J23 J33:J38 J61:J63 J3:J16 J75:J80 J29:J31 J40:J59 J65:J73" xr:uid="{94536AF8-B0B3-4690-A59B-64F66E932AAC}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5893,7 +5893,7 @@
   <dimension ref="A1:BS4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5975,202 +5975,202 @@
         <v>21</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AB1" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AE1" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="AF1" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="AG1" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="AE1" s="28" t="s">
-        <v>303</v>
-      </c>
-      <c r="AF1" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="AH1" s="15" t="s">
+      <c r="AI1" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="AI1" s="15" t="s">
+      <c r="AJ1" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="AJ1" s="15" t="s">
+      <c r="AK1" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="AK1" s="15" t="s">
+      <c r="AL1" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="AL1" s="15" t="s">
-        <v>271</v>
-      </c>
       <c r="AM1" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AN1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="AO1" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AP1" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="AQ1" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="AQ1" s="15" t="s">
-        <v>299</v>
-      </c>
       <c r="AR1" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="AS1" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="AS1" s="15" t="s">
+      <c r="AT1" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="AT1" s="15" t="s">
+      <c r="AU1" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="AU1" s="15" t="s">
+      <c r="AV1" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="AV1" s="15" t="s">
+      <c r="AW1" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="AW1" s="15" t="s">
+      <c r="AX1" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="AX1" s="15" t="s">
+      <c r="AY1" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="AY1" s="15" t="s">
+      <c r="AZ1" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="AZ1" s="15" t="s">
+      <c r="BA1" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="BA1" s="15" t="s">
+      <c r="BB1" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="BB1" s="15" t="s">
-        <v>317</v>
-      </c>
       <c r="BC1" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="BD1" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="BD1" s="15" t="s">
+      <c r="BE1" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="BE1" s="15" t="s">
+      <c r="BF1" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="BF1" s="15" t="s">
+      <c r="BG1" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="BG1" s="15" t="s">
+      <c r="BH1" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="BH1" s="15" t="s">
-        <v>329</v>
-      </c>
       <c r="BI1" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="BJ1" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="BJ1" s="15" t="s">
+      <c r="BK1" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="BK1" s="15" t="s">
+      <c r="BL1" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="BL1" s="15" t="s">
+      <c r="BM1" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="BN1" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="BM1" s="15" t="s">
-        <v>364</v>
-      </c>
-      <c r="BN1" s="15" t="s">
+      <c r="BO1" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="BO1" s="15" t="s">
+      <c r="BP1" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="BP1" s="15" t="s">
+      <c r="BQ1" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="BQ1" s="15" t="s">
+      <c r="BR1" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="BR1" s="15" t="s">
+      <c r="BS1" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="BS1" s="15" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:71" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -6178,10 +6178,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>22</v>
@@ -6190,118 +6190,118 @@
         <v>23</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G2" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="J2" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="K2" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="M2" s="24" t="s">
         <v>275</v>
       </c>
-      <c r="K2" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>302</v>
-      </c>
-      <c r="M2" s="24" t="s">
+      <c r="N2" s="24" t="s">
         <v>276</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="O2" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="P2" s="24" t="s">
         <v>277</v>
       </c>
-      <c r="O2" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="P2" s="24" t="s">
+      <c r="Q2" s="24" t="s">
         <v>278</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="R2" s="24" t="s">
         <v>279</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="S2" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="S2" s="24" t="s">
+      <c r="T2" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="T2" s="24" t="s">
+      <c r="U2" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="V2" s="24" t="s">
         <v>283</v>
       </c>
-      <c r="V2" s="24" t="s">
+      <c r="W2" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="X2" s="24" t="s">
         <v>284</v>
       </c>
-      <c r="W2" s="24" t="s">
-        <v>283</v>
-      </c>
-      <c r="X2" s="24" t="s">
+      <c r="Y2" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="Z2" s="24" t="s">
         <v>285</v>
       </c>
-      <c r="Y2" s="24" t="s">
+      <c r="AA2" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="AB2" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC2" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="AD2" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="AE2" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="AF2" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="AG2" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH2" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="AI2" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="AJ2" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="AK2" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="AL2" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="AM2" s="24" t="s">
         <v>354</v>
       </c>
-      <c r="Z2" s="24" t="s">
-        <v>286</v>
-      </c>
-      <c r="AA2" s="24" t="s">
-        <v>287</v>
-      </c>
-      <c r="AB2" s="24" t="s">
-        <v>288</v>
-      </c>
-      <c r="AC2" s="24" t="s">
-        <v>289</v>
-      </c>
-      <c r="AD2" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="AE2" s="24" t="s">
-        <v>304</v>
-      </c>
-      <c r="AF2" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="AG2" s="24" t="s">
-        <v>291</v>
-      </c>
-      <c r="AH2" s="24" t="s">
-        <v>341</v>
-      </c>
-      <c r="AI2" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="AJ2" s="24" t="s">
-        <v>369</v>
-      </c>
-      <c r="AK2" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="AL2" s="24" t="s">
-        <v>294</v>
-      </c>
-      <c r="AM2" s="24" t="s">
+      <c r="AN2" s="24" t="s">
         <v>355</v>
       </c>
-      <c r="AN2" s="24" t="s">
-        <v>356</v>
-      </c>
       <c r="AO2" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AP2" s="24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AQ2" s="24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AR2" s="12"/>
       <c r="AS2" s="12"/>
@@ -6317,13 +6317,13 @@
       <c r="BC2" s="12"/>
       <c r="BD2" s="12"/>
       <c r="BE2" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="BF2" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="BG2" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="BH2" s="26"/>
       <c r="BI2" s="12"/>
@@ -6343,7 +6343,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>43</v>
@@ -6380,22 +6380,22 @@
       <c r="AC3" s="12"/>
       <c r="AD3" s="12"/>
       <c r="AE3" s="24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AF3" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AG3" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH3" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="AI3" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="AH3" s="24" t="s">
-        <v>341</v>
-      </c>
-      <c r="AI3" s="24" t="s">
-        <v>292</v>
-      </c>
       <c r="AJ3" s="24" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AK3" s="12"/>
       <c r="AL3" s="12"/>
@@ -6435,10 +6435,10 @@
     </row>
     <row r="4" spans="1:71" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>43</v>
@@ -6488,88 +6488,88 @@
       <c r="AP4" s="12"/>
       <c r="AQ4" s="12"/>
       <c r="AR4" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="AS4" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="AS4" s="24" t="s">
+      <c r="AT4" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="AT4" s="24" t="s">
+      <c r="AU4" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="AV4" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="AU4" s="24" t="s">
+      <c r="AW4" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="AX4" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="AY4" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="AZ4" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="BA4" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="BB4" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="BC4" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="BD4" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="BE4" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="BF4" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="BG4" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="BH4" s="17" t="s">
+        <v>338</v>
+      </c>
+      <c r="BI4" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="BJ4" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="BK4" s="24" t="s">
+        <v>361</v>
+      </c>
+      <c r="BL4" s="24" t="s">
+        <v>361</v>
+      </c>
+      <c r="BM4" s="24" t="s">
+        <v>362</v>
+      </c>
+      <c r="BN4" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="AV4" s="24" t="s">
-        <v>321</v>
-      </c>
-      <c r="AW4" s="24" t="s">
+      <c r="BO4" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="BP4" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BQ4" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="BR4" s="24" t="s">
         <v>367</v>
       </c>
-      <c r="AX4" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="AY4" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="AZ4" s="24" t="s">
+      <c r="BS4" s="24" t="s">
         <v>322</v>
-      </c>
-      <c r="BA4" s="24" t="s">
-        <v>323</v>
-      </c>
-      <c r="BB4" s="24" t="s">
-        <v>365</v>
-      </c>
-      <c r="BC4" s="24" t="s">
-        <v>331</v>
-      </c>
-      <c r="BD4" s="24" t="s">
-        <v>332</v>
-      </c>
-      <c r="BE4" s="27" t="s">
-        <v>333</v>
-      </c>
-      <c r="BF4" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="BG4" s="17" t="s">
-        <v>338</v>
-      </c>
-      <c r="BH4" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="BI4" s="24" t="s">
-        <v>318</v>
-      </c>
-      <c r="BJ4" s="24" t="s">
-        <v>319</v>
-      </c>
-      <c r="BK4" s="24" t="s">
-        <v>362</v>
-      </c>
-      <c r="BL4" s="24" t="s">
-        <v>362</v>
-      </c>
-      <c r="BM4" s="24" t="s">
-        <v>363</v>
-      </c>
-      <c r="BN4" s="24" t="s">
-        <v>321</v>
-      </c>
-      <c r="BO4" s="24" t="s">
-        <v>321</v>
-      </c>
-      <c r="BP4" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="BQ4" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="BR4" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="BS4" s="24" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>